<commit_message>
finished exercises week 4
</commit_message>
<xml_diff>
--- a/04_exercises/cnn-ex1-stud.xlsx
+++ b/04_exercises/cnn-ex1-stud.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaron/workspace/mse_delearn/04_exercises/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDCFA9DB-7942-C944-972B-B6D4D9DF129A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBC47999-5562-E641-927B-E2F210CBF096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="860" windowWidth="34200" windowHeight="21380" xr2:uid="{8C63438D-D797-2F4D-8C3D-BC6A238C5B67}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="34200" windowHeight="21380" activeTab="1" xr2:uid="{8C63438D-D797-2F4D-8C3D-BC6A238C5B67}"/>
   </bookViews>
   <sheets>
     <sheet name="Ex 1-A" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>input</t>
   </si>
@@ -94,13 +94,52 @@
   </si>
   <si>
     <t>Ex 1b: 2D convolution</t>
+  </si>
+  <si>
+    <t>WARNING: Does not match input size</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>For which value of S&amp;P do we get a output of the same dimension as the input?</t>
+  </si>
+  <si>
+    <t>S1P1</t>
+  </si>
+  <si>
+    <t>Questions</t>
+  </si>
+  <si>
+    <t>Q: How many activation maps will be obtained?</t>
+  </si>
+  <si>
+    <t>A: 2, one for each filter</t>
+  </si>
+  <si>
+    <t>Q: With S=1 and P=0 what will be the dimension of the output volume?</t>
+  </si>
+  <si>
+    <t>A: 3x3x2</t>
+  </si>
+  <si>
+    <t>Q: With S=2 and P=0 what will be the dimension of the output volume?</t>
+  </si>
+  <si>
+    <t>A: 2x2x2</t>
+  </si>
+  <si>
+    <t>Q: Give a filter size, padding value and stride value that will preserve the spatial dimension of the output.</t>
+  </si>
+  <si>
+    <t>A: 3x3x3, Padding=1, Stride=1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -112,6 +151,13 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFFC000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -131,7 +177,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -172,11 +218,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -203,6 +262,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -517,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C3AA706-F46E-BE45-8FC6-3A8A2D1CEA6E}">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -621,31 +683,31 @@
       <c r="B10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="10">
         <f t="shared" ref="C10:I10" si="0">$C$6*C4+$D$6*D4+$E$6*E4+$C$7</f>
         <v>-1</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="10">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="10">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="10">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="10">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -655,19 +717,19 @@
       <c r="B11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="10">
         <f>$C$6*C4+$D$6*D4+$E$6*E4+$C$7</f>
         <v>-1</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="10">
         <f>$C$6*E4+$D$6*F4+$E$6*G4+$C$7</f>
         <v>4</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="10">
         <f>$C$6*G4+$D$6*H4+$E$6*I4+$C$7</f>
         <v>1</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="10">
         <f>$C$6*I4+$D$6*J4+$E$6*K4+$C$7</f>
         <v>3</v>
       </c>
@@ -677,13 +739,16 @@
       <c r="B12" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="11">
         <f>$C$6*C4+$D$6*D4+$E$6*E4+$C$7</f>
         <v>-1</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="11">
         <f>$C$6*G4+$D$6*H4+$E$6*I4+$C$7</f>
         <v>1</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -691,39 +756,39 @@
       <c r="B13" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="10">
         <f>$C$6*B4+$D$6*C4+$E$6*D4+$C$7</f>
         <v>6</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="10">
         <f t="shared" ref="D13:J13" si="1">$C$6*C4+$D$6*D4+$E$6*E4+$C$7</f>
         <v>-1</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="10">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="10">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="10">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="10">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="10">
         <f>$C$6*H4+$D$6*I4+$E$6*J4+$C$7</f>
         <v>0</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="10">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="10">
         <f>$C$6*J4+$D$6*K4+$E$6*L4+$C$7</f>
         <v>6</v>
       </c>
@@ -733,21 +798,36 @@
       <c r="B14" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="10">
         <f>$C$6*B4+$D$6*C4+$E$6*D4+$C$7</f>
         <v>6</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="10">
         <f>$C$6*F4+$D$6*G4+$E$6*H4+$C$7</f>
         <v>6</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="10">
         <f>$C$6*J4+$D$6*K4+$E$6*L4+$C$7</f>
         <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -761,10 +841,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D308E945-0386-A246-9572-FC8DE175F97D}">
-  <dimension ref="A1:V22"/>
+  <dimension ref="A1:AB22"/>
   <sheetViews>
-    <sheetView zoomScale="169" workbookViewId="0">
-      <selection activeCell="X9" sqref="X9"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="AD15" sqref="AD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -775,7 +855,7 @@
     <col min="28" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>18</v>
       </c>
@@ -784,7 +864,7 @@
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
     </row>
-    <row r="2" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K2" s="3" t="s">
         <v>6</v>
       </c>
@@ -795,8 +875,11 @@
       <c r="T2" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AB2" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -844,8 +927,11 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="4" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AB3" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D4" s="2">
         <v>0</v>
       </c>
@@ -884,8 +970,11 @@
         <f t="shared" ref="V4:V5" si="3">SUMPRODUCT(F4:G5,$K$3:$L$4)+SUMPRODUCT(F10:G11,$K$6:$L$7)+SUMPRODUCT(F16:G17,$K$9:$L$10)+$L$12</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AB4" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D5" s="2">
         <v>1</v>
       </c>
@@ -913,8 +1002,11 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AB5" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D6" s="2">
         <v>0</v>
       </c>
@@ -943,8 +1035,11 @@
       <c r="P6" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AB6" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -973,8 +1068,11 @@
         <f>SUMPRODUCT(F3:G4,$O$3:$P$4)+SUMPRODUCT(F9:G10,$O$6:$P$7)+SUMPRODUCT(F15:G16,$O$9:$P$10)+$P$12</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AB7" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="T8" s="2">
         <f t="shared" ref="T8:T9" si="4">SUMPRODUCT(D4:E5,$O$3:$P$4)+SUMPRODUCT(D10:E11,$O$6:$P$7)+SUMPRODUCT(D16:E17,$O$9:$P$10)+$P$12</f>
         <v>4</v>
@@ -987,8 +1085,11 @@
         <f t="shared" ref="V8:V9" si="6">SUMPRODUCT(F4:G5,$O$3:$P$4)+SUMPRODUCT(F10:G11,$O$6:$P$7)+SUMPRODUCT(F16:G17,$O$9:$P$10)+$P$12</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AB8" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
@@ -1032,8 +1133,11 @@
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AB9" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D10" s="2">
         <v>0</v>
       </c>
@@ -1059,8 +1163,11 @@
       <c r="P10" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AB10" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D11" s="2">
         <v>1</v>
       </c>
@@ -1075,7 +1182,7 @@
       </c>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D12" s="2">
         <v>2</v>
       </c>
@@ -1102,14 +1209,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
@@ -1127,7 +1234,7 @@
       </c>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D16" s="2">
         <v>0</v>
       </c>

</xml_diff>